<commit_message>
[TASK] use attributes import id in examples. Create example for attribute files
</commit_message>
<xml_diff>
--- a/Resources/Private/ExampleData/products.xlsx
+++ b/Resources/Private/ExampleData/products.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -76,6 +76,12 @@
     <t xml:space="preserve">Meta description</t>
   </si>
   <si>
+    <t xml:space="preserve">Fal files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fal images</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chevrolet Pick up</t>
   </si>
   <si>
@@ -112,6 +118,9 @@
     <t xml:space="preserve">test-document-pdf.pdf</t>
   </si>
   <si>
+    <t xml:space="preserve">bicycle_cannondale_black.jpg,bicycle_cannondale_red.jpg,bicycle_cannondale_white.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">BMW Roadster</t>
   </si>
   <si>
@@ -151,10 +160,10 @@
     <t xml:space="preserve">White,Red</t>
   </si>
   <si>
-    <t xml:space="preserve">bicycle_cannondale_black.jpg,bicycle_cannondale_red.jpg,bicycle_cannondale_white.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">445566,112233 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bicycle_cannondale_black.jpg</t>
   </si>
 </sst>
 </file>
@@ -240,12 +249,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -255,10 +264,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T4" activeCellId="0" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -321,46 +330,52 @@
       <c r="R1" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>112233</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="0" t="n">
@@ -370,71 +385,77 @@
         <v>778899</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>445566</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="N3" s="1" t="n">
         <v>112233</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>778899</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>18</v>
@@ -443,10 +464,16 @@
         <v>0</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>